<commit_message>
work on pdinit and db structure
</commit_message>
<xml_diff>
--- a/notes/postdoc system database structure.xlsx
+++ b/notes/postdoc system database structure.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12CBBA2-C11D-464D-87C7-C17ADDF37553}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B11EB7-5677-4A30-8052-5FED2FC48597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="1" r:id="rId1"/>
     <sheet name="archive" sheetId="2" r:id="rId2"/>
+    <sheet name="resources" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="103">
   <si>
     <t>table</t>
   </si>
@@ -145,12 +146,6 @@
     <t>preferences</t>
   </si>
   <si>
-    <t>prefid</t>
-  </si>
-  <si>
-    <t>INTEGER PRIMARY KEY</t>
-  </si>
-  <si>
     <t>section</t>
   </si>
   <si>
@@ -178,21 +173,12 @@
     <t>docid</t>
   </si>
   <si>
-    <t>initstamp</t>
-  </si>
-  <si>
-    <t>inituser</t>
-  </si>
-  <si>
     <t>stage</t>
   </si>
   <si>
     <t>stamp</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>app</t>
   </si>
   <si>
@@ -215,6 +201,141 @@
   </si>
   <si>
     <t>&lt;user metadata&gt;</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (section , key)</t>
+  </si>
+  <si>
+    <t>pdsyslog</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>archives</t>
+  </si>
+  <si>
+    <t>datasets</t>
+  </si>
+  <si>
+    <t>accesstokens</t>
+  </si>
+  <si>
+    <t>applications</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>friendlyname</t>
+  </si>
+  <si>
+    <t>passwd</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>tokens</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>BOOLEAN NOT NULL</t>
+  </si>
+  <si>
+    <t>envelope</t>
+  </si>
+  <si>
+    <t>envid</t>
+  </si>
+  <si>
+    <t>workflow</t>
+  </si>
+  <si>
+    <t>envelopeid</t>
+  </si>
+  <si>
+    <t>sysenvelope</t>
+  </si>
+  <si>
+    <t>contentid_main_md5</t>
+  </si>
+  <si>
+    <t>contentid_aux_md5</t>
+  </si>
+  <si>
+    <t>storagepool</t>
+  </si>
+  <si>
+    <t>pdusers</t>
+  </si>
+  <si>
+    <t>pdgroups</t>
+  </si>
+  <si>
+    <t>syslog</t>
+  </si>
+  <si>
+    <t>fieldnames</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>resourcename</t>
+  </si>
+  <si>
+    <t>resourcetype</t>
+  </si>
+  <si>
+    <t>archive</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>comma delimited</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>also apply to content</t>
+  </si>
+  <si>
+    <t>pgusers</t>
+  </si>
+  <si>
+    <t>BIGINT REFERENCES archive.sysenvelope(envid)</t>
   </si>
 </sst>
 </file>
@@ -286,11 +407,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,17 +905,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42085D-1F11-446D-9971-ADB34FF5C9D9}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
@@ -825,12 +948,12 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -838,15 +961,15 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -854,7 +977,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -862,7 +985,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -870,7 +993,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
@@ -878,18 +1001,15 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -897,81 +1017,726 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
+      <c r="B15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125F4650-A109-4B7E-84D7-96E78511890D}">
+  <dimension ref="A1:G69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>62</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" t="s">
+        <v>91</v>
+      </c>
+      <c r="G60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on pdinit and system db structure
</commit_message>
<xml_diff>
--- a/notes/postdoc system database structure.xlsx
+++ b/notes/postdoc system database structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B11EB7-5677-4A30-8052-5FED2FC48597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BC1C09-45EC-4BA8-93E6-72F369239382}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6750" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="104">
   <si>
     <t>table</t>
   </si>
@@ -311,9 +311,6 @@
     <t>read</t>
   </si>
   <si>
-    <t>create</t>
-  </si>
-  <si>
     <t>update</t>
   </si>
   <si>
@@ -323,19 +320,25 @@
     <t>execute</t>
   </si>
   <si>
-    <t>comma delimited</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
-    <t>also apply to content</t>
-  </si>
-  <si>
     <t>pgusers</t>
   </si>
   <si>
     <t>BIGINT REFERENCES archive.sysenvelope(envid)</t>
+  </si>
+  <si>
+    <t>pggroups</t>
+  </si>
+  <si>
+    <t>ALSO applies to content</t>
+  </si>
+  <si>
+    <t>createnew</t>
+  </si>
+  <si>
+    <t>TEXT REFERENCES resources.archives(name)</t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42085D-1F11-446D-9971-ADB34FF5C9D9}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
@@ -1028,7 +1031,7 @@
         <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,11 +1185,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125F4650-A109-4B7E-84D7-96E78511890D}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1222,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
@@ -1270,7 +1273,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>65</v>
@@ -1466,15 +1469,15 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
@@ -1490,188 +1493,185 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" t="s">
-        <v>26</v>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" t="s">
-        <v>26</v>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>64</v>
-      </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
       </c>
-      <c r="D53" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" t="s">
-        <v>26</v>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>63</v>
-      </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" t="s">
+        <v>91</v>
+      </c>
+      <c r="G59" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
-      <c r="E60" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" t="s">
-        <v>91</v>
-      </c>
-      <c r="G60" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
         <v>74</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
         <v>74</v>
@@ -1703,39 +1703,28 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D67" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
-        <v>74</v>
-      </c>
-      <c r="D68" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
work on db structure
</commit_message>
<xml_diff>
--- a/notes/postdoc system database structure.xlsx
+++ b/notes/postdoc system database structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BC1C09-45EC-4BA8-93E6-72F369239382}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50B32EB-F443-415B-93B9-C8587CF8143C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6750" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
   <si>
     <t>table</t>
   </si>
@@ -152,21 +152,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>value1</t>
-  </si>
-  <si>
-    <t>value2</t>
-  </si>
-  <si>
-    <t>value3</t>
-  </si>
-  <si>
-    <t>value4</t>
-  </si>
-  <si>
-    <t>value5</t>
-  </si>
-  <si>
     <t>documents</t>
   </si>
   <si>
@@ -263,12 +248,6 @@
     <t>workflow</t>
   </si>
   <si>
-    <t>envelopeid</t>
-  </si>
-  <si>
-    <t>sysenvelope</t>
-  </si>
-  <si>
     <t>contentid_main_md5</t>
   </si>
   <si>
@@ -339,6 +318,12 @@
   </si>
   <si>
     <t>TEXT REFERENCES resources.archives(name)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>envelopes</t>
   </si>
 </sst>
 </file>
@@ -363,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +364,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,12 +407,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,11 +907,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42085D-1F11-446D-9971-ADB34FF5C9D9}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +963,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -972,210 +971,186 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>58</v>
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>56</v>
+      <c r="B24" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>81</v>
+      <c r="B25" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>59</v>
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>57</v>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
+      <c r="B30" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>65</v>
+      <c r="B31" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>77</v>
+      <c r="B32" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>48</v>
+      <c r="B33" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>12</v>
+      <c r="B34" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>51</v>
+      <c r="B38" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1187,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125F4650-A109-4B7E-84D7-96E78511890D}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -1222,10 +1197,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1233,7 +1208,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1249,7 +1224,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1257,7 +1232,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>26</v>
@@ -1265,7 +1240,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -1273,10 +1248,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -1284,7 +1259,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -1300,7 +1275,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>26</v>
@@ -1308,7 +1283,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1316,10 +1291,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1327,7 +1302,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -1335,7 +1310,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1351,7 +1326,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
         <v>26</v>
@@ -1359,15 +1334,15 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
@@ -1375,7 +1350,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -1383,7 +1358,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
@@ -1391,10 +1366,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
@@ -1402,7 +1377,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1418,15 +1393,15 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>26</v>
@@ -1434,7 +1409,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>26</v>
@@ -1442,10 +1417,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -1453,7 +1428,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1469,7 +1444,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
@@ -1477,7 +1452,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -1485,7 +1460,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
@@ -1493,7 +1468,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -1501,10 +1476,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
@@ -1512,7 +1487,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1528,15 +1503,15 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -1544,7 +1519,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
         <v>26</v>
@@ -1552,10 +1527,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
@@ -1563,7 +1538,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1579,15 +1554,15 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -1595,7 +1570,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -1603,10 +1578,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
@@ -1614,7 +1589,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1630,32 +1605,32 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F59" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G59" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1663,47 +1638,47 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C66" t="s">
         <v>26</v>
@@ -1711,18 +1686,18 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C68" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
work on system db structure
</commit_message>
<xml_diff>
--- a/notes/postdoc system database structure.xlsx
+++ b/notes/postdoc system database structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50B32EB-F443-415B-93B9-C8587CF8143C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B449555-A722-4C8D-996B-924E63F151A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7650" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="105">
   <si>
     <t>table</t>
   </si>
@@ -248,12 +248,6 @@
     <t>workflow</t>
   </si>
   <si>
-    <t>contentid_main_md5</t>
-  </si>
-  <si>
-    <t>contentid_aux_md5</t>
-  </si>
-  <si>
     <t>storagepool</t>
   </si>
   <si>
@@ -324,6 +318,30 @@
   </si>
   <si>
     <t>envelopes</t>
+  </si>
+  <si>
+    <t>contenthash_main</t>
+  </si>
+  <si>
+    <t>contenthash_aux</t>
+  </si>
+  <si>
+    <t>errormessage</t>
+  </si>
+  <si>
+    <t>errorcode</t>
+  </si>
+  <si>
+    <t>documents_historical</t>
+  </si>
+  <si>
+    <t>objid</t>
+  </si>
+  <si>
+    <t>BIGINT REFERENCES archive.documents(docid)</t>
+  </si>
+  <si>
+    <t>BIGINT REFERENCES archive.envelopes(envid)</t>
   </si>
 </sst>
 </file>
@@ -907,16 +925,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42085D-1F11-446D-9971-ADB34FF5C9D9}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
@@ -963,7 +981,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -998,7 +1016,7 @@
         <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,92 +1087,250 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
         <v>71</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C53" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="6" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1197,7 +1373,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -1240,7 +1416,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -1248,7 +1424,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -1283,7 +1459,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1291,7 +1467,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
@@ -1358,7 +1534,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
@@ -1366,7 +1542,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -1409,7 +1585,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
         <v>26</v>
@@ -1444,7 +1620,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
@@ -1460,7 +1636,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
@@ -1468,7 +1644,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -1503,15 +1679,15 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -1519,7 +1695,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
         <v>26</v>
@@ -1562,7 +1738,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -1570,7 +1746,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -1613,24 +1789,24 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F59" t="s">
         <v>82</v>
       </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="G59" t="s">
         <v>83</v>
-      </c>
-      <c r="F59" t="s">
-        <v>84</v>
-      </c>
-      <c r="G59" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1638,7 +1814,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C61" t="s">
         <v>69</v>
@@ -1646,7 +1822,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C62" t="s">
         <v>69</v>
@@ -1654,7 +1830,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C63" t="s">
         <v>69</v>
@@ -1662,7 +1838,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
         <v>69</v>
@@ -1670,7 +1846,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C65" t="s">
         <v>69</v>
@@ -1678,7 +1854,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C66" t="s">
         <v>26</v>
@@ -1686,18 +1862,18 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C67" t="s">
         <v>69</v>
       </c>
       <c r="D67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C68" t="s">
         <v>26</v>

</xml_diff>